<commit_message>
update email feedback and unit test
</commit_message>
<xml_diff>
--- a/_unittests/ut_automation_students/data/groupes_eleves_pitch.xlsx
+++ b/_unittests/ut_automation_students/data/groupes_eleves_pitch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="0" windowWidth="19560" windowHeight="7740"/>
+    <workbookView xWindow="15810" yWindow="0" windowWidth="19560" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="pitch" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>ok</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Mail</t>
+  </si>
+  <si>
+    <t>bbb.aaa@ensae.fr</t>
+  </si>
+  <si>
+    <t>ccc.aba@ensae.fr</t>
+  </si>
+  <si>
+    <t>uuu.vvv@ensae.fr</t>
   </si>
 </sst>
 </file>
@@ -503,7 +512,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +547,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -547,6 +558,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -564,6 +578,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -657,8 +674,13 @@
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update code to automatically send feedback
</commit_message>
<xml_diff>
--- a/_unittests/ut_automation_students/data/groupes_eleves_pitch.xlsx
+++ b/_unittests/ut_automation_students/data/groupes_eleves_pitch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="0" windowWidth="19560" windowHeight="7740"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="19560" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="pitch" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>uuu.vvv@ensae.fr</t>
+  </si>
+  <si>
+    <t>Nom</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,10 +528,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>22</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>

</xml_diff>